<commit_message>
comit versao para testes
</commit_message>
<xml_diff>
--- a/controle_contratos/Tabela_Gestores_Fiscais.xlsx
+++ b/controle_contratos/Tabela_Gestores_Fiscais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/Programa PYQT6/pyqt6/controle_contratos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_23F921ED65A349372D2D4CD68DDDEC694DFA4A78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C70E28ED-8357-454E-96DC-E8441C2E461D}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_23F921EDD1234E30692D4C261D7D54E979F84AF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F34EE89-4078-481A-A1B0-49C4E3996125}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="163">
   <si>
     <t>Número</t>
   </si>
@@ -37,189 +37,201 @@
     <t>Setor</t>
   </si>
   <si>
+    <t>Posto/Graduação Gestor</t>
+  </si>
+  <si>
     <t>Gestor</t>
   </si>
   <si>
+    <t>Posto/Graduação Gestor Substituto</t>
+  </si>
+  <si>
     <t>Gestor Substituto</t>
   </si>
   <si>
+    <t>Posto/Graduação Fiscal</t>
+  </si>
+  <si>
     <t>Fiscal</t>
   </si>
   <si>
+    <t>Posto/Graduação Fiscal Substituto</t>
+  </si>
+  <si>
     <t>Fiscal Substituto</t>
   </si>
   <si>
+    <t>87000/24-002/00</t>
+  </si>
+  <si>
+    <t>87000/19-033/00</t>
+  </si>
+  <si>
+    <t>87000/22-007/00</t>
+  </si>
+  <si>
+    <t>87000/22-032/00</t>
+  </si>
+  <si>
+    <t>87000/21-084/00</t>
+  </si>
+  <si>
+    <t>87000/21-085/00</t>
+  </si>
+  <si>
+    <t>87000/21-086/00</t>
+  </si>
+  <si>
+    <t>87000/23-073/00</t>
+  </si>
+  <si>
+    <t>87000/21-135/00</t>
+  </si>
+  <si>
+    <t>87000/21-120/00</t>
+  </si>
+  <si>
+    <t>87000/23-087/00</t>
+  </si>
+  <si>
+    <t>87000/21-140/00</t>
+  </si>
+  <si>
+    <t>87000/23-099/00</t>
+  </si>
+  <si>
+    <t>87000/23-108/00</t>
+  </si>
+  <si>
+    <t>87000/23-088/00</t>
+  </si>
+  <si>
+    <t>87000/21-080/00</t>
+  </si>
+  <si>
+    <t>87000/20-082/00</t>
+  </si>
+  <si>
+    <t>87000/23-121/00</t>
+  </si>
+  <si>
+    <t>87000/23-115/00</t>
+  </si>
+  <si>
+    <t>87000/20-080/00</t>
+  </si>
+  <si>
+    <t>87000/21-156/00</t>
+  </si>
+  <si>
+    <t>87000/19-058/00</t>
+  </si>
+  <si>
+    <t>87000/21-109/00</t>
+  </si>
+  <si>
+    <t>87000/19-059/00</t>
+  </si>
+  <si>
+    <t>87000/17-1531/00</t>
+  </si>
+  <si>
     <t>87000/17-1532/00</t>
   </si>
   <si>
-    <t>87000/21-135/00</t>
-  </si>
-  <si>
-    <t>87000/23-073/00</t>
-  </si>
-  <si>
-    <t>87000/21-120/00</t>
-  </si>
-  <si>
-    <t>87000/21-080/00</t>
-  </si>
-  <si>
-    <t>87000/21-109/00</t>
-  </si>
-  <si>
-    <t>87000/21-086/00</t>
-  </si>
-  <si>
-    <t>87000/17-1531/00</t>
-  </si>
-  <si>
-    <t>87000/21-085/00</t>
-  </si>
-  <si>
-    <t>87000/21-084/00</t>
-  </si>
-  <si>
-    <t>87000/22-032/00</t>
-  </si>
-  <si>
-    <t>87000/23-087/00</t>
-  </si>
-  <si>
-    <t>87000/21-140/00</t>
-  </si>
-  <si>
-    <t>87000/21-005/00</t>
-  </si>
-  <si>
-    <t>87000/23-099/00</t>
-  </si>
-  <si>
-    <t>87000/23-108/00</t>
-  </si>
-  <si>
-    <t>87000/23-088/00</t>
-  </si>
-  <si>
-    <t>87000/20-080/00</t>
-  </si>
-  <si>
-    <t>87000/20-082/00</t>
+    <t>87000/19-057/00</t>
+  </si>
+  <si>
+    <t>87000/21-154/00</t>
   </si>
   <si>
     <t>87000/22-009/00</t>
   </si>
   <si>
-    <t>87000/21-154/00</t>
-  </si>
-  <si>
-    <t>87000/19-057/00</t>
-  </si>
-  <si>
-    <t>87000/19-059/00</t>
-  </si>
-  <si>
-    <t>87000/19-058/00</t>
-  </si>
-  <si>
-    <t>87000/21-156/00</t>
-  </si>
-  <si>
-    <t>87000/23-115/00</t>
-  </si>
-  <si>
-    <t>87000/23-121/00</t>
-  </si>
-  <si>
-    <t>87000/22-007/00</t>
-  </si>
-  <si>
-    <t>87000/19-033/00</t>
+    <t>87000/23-032/00</t>
+  </si>
+  <si>
+    <t>87000/23-036/00</t>
+  </si>
+  <si>
+    <t>87000/23-044/00</t>
+  </si>
+  <si>
+    <t>87000/23-045/00</t>
+  </si>
+  <si>
+    <t>87000/23-033/00</t>
+  </si>
+  <si>
+    <t>87000/23-035/00</t>
   </si>
   <si>
     <t>87000/23-048/00</t>
   </si>
   <si>
+    <t>87000/23-037/00</t>
+  </si>
+  <si>
+    <t>87000/23-041/00</t>
+  </si>
+  <si>
+    <t>87000/23-040/00</t>
+  </si>
+  <si>
+    <t>87000/23-046/00</t>
+  </si>
+  <si>
+    <t>87000/23-043/00</t>
+  </si>
+  <si>
+    <t>87000/23-042/00</t>
+  </si>
+  <si>
+    <t>87000/23-072/00</t>
+  </si>
+  <si>
+    <t>87000/23-076/00</t>
+  </si>
+  <si>
+    <t>87000/23-074/00</t>
+  </si>
+  <si>
+    <t>87000/23-082/00</t>
+  </si>
+  <si>
+    <t>87000/23-081/00</t>
+  </si>
+  <si>
+    <t>87000/23-031/00</t>
+  </si>
+  <si>
+    <t>87000/23-075/00</t>
+  </si>
+  <si>
+    <t>87000/23-078/00</t>
+  </si>
+  <si>
+    <t>87000/23-079/00</t>
+  </si>
+  <si>
+    <t>87000/23-080/00</t>
+  </si>
+  <si>
+    <t>87000/23-084/00</t>
+  </si>
+  <si>
+    <t>87000/23-085/00</t>
+  </si>
+  <si>
+    <t>87000/23-086/00</t>
+  </si>
+  <si>
+    <t>87000/23-098/00</t>
+  </si>
+  <si>
     <t>87000/24-003/00</t>
   </si>
   <si>
-    <t>87000/23-042/00</t>
-  </si>
-  <si>
-    <t>87000/23-036/00</t>
-  </si>
-  <si>
-    <t>87000/23-032/00</t>
-  </si>
-  <si>
-    <t>87000/23-043/00</t>
-  </si>
-  <si>
-    <t>87000/23-045/00</t>
-  </si>
-  <si>
-    <t>87000/23-035/00</t>
-  </si>
-  <si>
-    <t>87000/23-041/00</t>
-  </si>
-  <si>
-    <t>87000/23-040/00</t>
-  </si>
-  <si>
-    <t>87000/23-033/00</t>
-  </si>
-  <si>
-    <t>87000/23-044/00</t>
-  </si>
-  <si>
-    <t>87000/23-074/00</t>
-  </si>
-  <si>
-    <t>87000/23-046/00</t>
-  </si>
-  <si>
-    <t>87000/23-072/00</t>
-  </si>
-  <si>
-    <t>87000/23-076/00</t>
-  </si>
-  <si>
-    <t>87000/23-031/00</t>
-  </si>
-  <si>
-    <t>87000/23-082/00</t>
-  </si>
-  <si>
-    <t>87000/23-081/00</t>
-  </si>
-  <si>
-    <t>87000/23-075/00</t>
-  </si>
-  <si>
-    <t>87000/23-078/00</t>
-  </si>
-  <si>
-    <t>87000/23-079/00</t>
-  </si>
-  <si>
-    <t>87000/23-080/00</t>
-  </si>
-  <si>
-    <t>87000/23-084/00</t>
-  </si>
-  <si>
-    <t>87000/23-085/00</t>
-  </si>
-  <si>
-    <t>87000/23-086/00</t>
-  </si>
-  <si>
-    <t>87000/23-098/00</t>
-  </si>
-  <si>
-    <t>87000/23-037/00</t>
-  </si>
-  <si>
     <t>87000/23-034/00</t>
   </si>
   <si>
@@ -229,232 +241,244 @@
     <t>Ata</t>
   </si>
   <si>
+    <t>UEDAMA COMERCIO DE PRODUTOS A</t>
+  </si>
+  <si>
+    <t>LUCIANO GONÇALVES BORBA ASSUNÇÃO</t>
+  </si>
+  <si>
+    <t>COPY LINE COMERCIO E SERVICOS</t>
+  </si>
+  <si>
+    <t>NP3 COMERCIO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>ADTEL FACILITIES LTDA</t>
+  </si>
+  <si>
+    <t>HEIMAR-CONSTRUCOES E SERVICOS</t>
+  </si>
+  <si>
+    <t>TECNICALL ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>NORESA NOVO RIO ENERGIA E SER</t>
+  </si>
+  <si>
+    <t>VIVACE FISIOTERAPIA &amp; MEDICIN</t>
+  </si>
+  <si>
+    <t>CLIAMA CLINICA DE ATENDIMENTO</t>
+  </si>
+  <si>
+    <t>MCR SISTEMAS E CONSULTORIA LT</t>
+  </si>
+  <si>
+    <t>PRATICAR CENTRO DE TREINAMENT</t>
+  </si>
+  <si>
+    <t>ELP COMERCIO DE EQUIPAMENTOS</t>
+  </si>
+  <si>
+    <t>OVER ELEVADORES LTDA</t>
+  </si>
+  <si>
+    <t>CLARO S.A.</t>
+  </si>
+  <si>
+    <t>INTEGRAR - INSTITUTO DE REABI</t>
+  </si>
+  <si>
+    <t>STAR LOCACAO DE SERVICOS GERA</t>
+  </si>
+  <si>
+    <t>ABRIGO DO MARINHEIRO</t>
+  </si>
+  <si>
+    <t>SEGUROS SURA S.A.</t>
+  </si>
+  <si>
+    <t>PALCO LOCACAO LTDA</t>
+  </si>
+  <si>
+    <t>UNICA SERVICOS EM SAUDE LTDA</t>
+  </si>
+  <si>
+    <t>CAIXA ECONOMICA FEDERAL</t>
+  </si>
+  <si>
+    <t>ANDRACON SERVICOS GERAIS LTDA</t>
+  </si>
+  <si>
+    <t>BANCO SANTANDER (BRASIL) S.A.</t>
+  </si>
+  <si>
     <t>NEOENERGIA DISTRIBUICAO BRASI</t>
   </si>
   <si>
-    <t>VIVACE FISIOTERAPIA &amp; MEDICIN</t>
-  </si>
-  <si>
-    <t>NORESA NOVO RIO ENERGIA E SER</t>
-  </si>
-  <si>
-    <t>CLIAMA CLINICA DE ATENDIMENTO</t>
-  </si>
-  <si>
-    <t>INTEGRAR - INSTITUTO DE REABI</t>
-  </si>
-  <si>
-    <t>ANDRACON SERVICOS GERAIS LTDA</t>
-  </si>
-  <si>
-    <t>TECNICALL ENGENHARIA LTDA</t>
-  </si>
-  <si>
-    <t>HEIMAR-CONSTRUCOES E SERVICOS</t>
-  </si>
-  <si>
-    <t>ADTEL FACILITIES LTDA</t>
-  </si>
-  <si>
-    <t>NP3 COMERCIO E SERVICOS LTDA</t>
-  </si>
-  <si>
-    <t>MCR SISTEMAS E CONSULTORIA LT</t>
-  </si>
-  <si>
-    <t>PRATICAR CENTRO DE TREINAMENT</t>
-  </si>
-  <si>
-    <t>FORTT DO BRASIL LTDA</t>
-  </si>
-  <si>
-    <t>ELP COMERCIO DE EQUIPAMENTOS</t>
-  </si>
-  <si>
-    <t>OVER ELEVADORES LTDA</t>
-  </si>
-  <si>
-    <t>CLARO S.A.</t>
-  </si>
-  <si>
-    <t>PALCO LOCACAO LTDA</t>
-  </si>
-  <si>
-    <t>STAR LOCACAO DE SERVICOS GERA</t>
+    <t>BANCO BRADESCO S.A.</t>
+  </si>
+  <si>
+    <t>MARCIO ANDERSON RODRIGUES COM</t>
   </si>
   <si>
     <t>ALFA E OMEGA  SERVICOS TERCEI</t>
   </si>
   <si>
-    <t>MARCIO ANDERSON RODRIGUES COM</t>
-  </si>
-  <si>
-    <t>BANCO BRADESCO S.A.</t>
-  </si>
-  <si>
-    <t>BANCO SANTANDER (BRASIL) S.A.</t>
-  </si>
-  <si>
-    <t>CAIXA ECONOMICA FEDERAL</t>
-  </si>
-  <si>
-    <t>UNICA SERVICOS EM SAUDE LTDA</t>
-  </si>
-  <si>
-    <t>SEGUROS SURA S.A.</t>
-  </si>
-  <si>
-    <t>ABRIGO DO MARINHEIRO</t>
-  </si>
-  <si>
-    <t>COPY LINE COMERCIO E SERVICOS</t>
-  </si>
-  <si>
-    <t>LUCIANO GONÇALVES BORBA ASSUNÇÃO</t>
+    <t>LER - LIVRARIA E PAPELARIA LT</t>
+  </si>
+  <si>
+    <t>LG COMERCIO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>THIAGO CAETANIO DA SILVA 0549</t>
+  </si>
+  <si>
+    <t>DAIANE DOS SANTOS MARTINS 133</t>
+  </si>
+  <si>
+    <t>AMAZONAS COMERCIO DE ADESIVOS</t>
+  </si>
+  <si>
+    <t>VS - VIEIRA &amp; SANTOS COMERCIO</t>
+  </si>
+  <si>
+    <t>RX PROMOCAO DE VENDAS E COMER</t>
+  </si>
+  <si>
+    <t>DM COMERCIAL IMPORTADORA E EX</t>
+  </si>
+  <si>
+    <t>RAFA PAPER DISTRIBUIDORA LTDA</t>
+  </si>
+  <si>
+    <t>ART PAPER INDUSTRIA E COMERCI</t>
+  </si>
+  <si>
+    <t>ALEGRENSE DISTRIBUIDORA E REP</t>
+  </si>
+  <si>
+    <t>SMART SOLUTIONS - SOLUCOES IN</t>
+  </si>
+  <si>
+    <t>M&amp;M IMPORTACAO E ECOMMERCE DE</t>
+  </si>
+  <si>
+    <t>ARCANJO TELECOMUNICACOES E IN</t>
+  </si>
+  <si>
+    <t>NOVA ERA TECNOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t>REPREMIG REPRESENTACAO E COME</t>
+  </si>
+  <si>
+    <t>LAZARO BEZERRA SOARES</t>
+  </si>
+  <si>
+    <t>OKAY TECHNOLOGY COMERCIO DO B</t>
+  </si>
+  <si>
+    <t>BACKUP MANUTENCAO E DISTRIBUI</t>
+  </si>
+  <si>
+    <t>NOVA MIX LTDA</t>
+  </si>
+  <si>
+    <t>DANIEL TAVARES DE GOES</t>
+  </si>
+  <si>
+    <t>ALPHA ELETRONICOS DO BRASIL L</t>
+  </si>
+  <si>
+    <t>J L PEREIRA ARCHILLA</t>
+  </si>
+  <si>
+    <t>GLOBAL DISTRIBUICAO DE BENS D</t>
   </si>
   <si>
     <t>COMERCIAL MINAS BRASILIA LTDA</t>
   </si>
   <si>
-    <t>SMART SOLUTIONS - SOLUCOES IN</t>
-  </si>
-  <si>
-    <t>LG COMERCIO E SERVICOS LTDA</t>
-  </si>
-  <si>
-    <t>LER - LIVRARIA E PAPELARIA LT</t>
-  </si>
-  <si>
-    <t>ALEGRENSE DISTRIBUIDORA E REP</t>
-  </si>
-  <si>
-    <t>DAIANE DOS SANTOS MARTINS 133</t>
-  </si>
-  <si>
-    <t>VS - VIEIRA &amp; SANTOS COMERCIO</t>
-  </si>
-  <si>
-    <t>DM COMERCIAL IMPORTADORA E EX</t>
-  </si>
-  <si>
-    <t>RAFA PAPER DISTRIBUIDORA LTDA</t>
-  </si>
-  <si>
-    <t>AMAZONAS COMERCIO DE ADESIVOS</t>
-  </si>
-  <si>
-    <t>THIAGO CAETANIO DA SILVA 0549</t>
-  </si>
-  <si>
-    <t>ARCANJO TELECOMUNICACOES E IN</t>
-  </si>
-  <si>
-    <t>ART PAPER INDUSTRIA E COMERCI</t>
-  </si>
-  <si>
-    <t>M&amp;M IMPORTACAO E ECOMMERCE DE</t>
-  </si>
-  <si>
-    <t>LAZARO BEZERRA SOARES</t>
-  </si>
-  <si>
-    <t>NOVA ERA TECNOLOGIA LTDA</t>
-  </si>
-  <si>
-    <t>REPREMIG REPRESENTACAO E COME</t>
-  </si>
-  <si>
-    <t>OKAY TECHNOLOGY COMERCIO DO B</t>
-  </si>
-  <si>
-    <t>BACKUP MANUTENCAO E DISTRIBUI</t>
-  </si>
-  <si>
-    <t>NOVA MIX LTDA</t>
-  </si>
-  <si>
-    <t>DANIEL TAVARES DE GOES</t>
-  </si>
-  <si>
-    <t>ALPHA ELETRONICOS DO BRASIL L</t>
-  </si>
-  <si>
-    <t>J L PEREIRA ARCHILLA</t>
-  </si>
-  <si>
-    <t>GLOBAL DISTRIBUICAO DE BENS D</t>
-  </si>
-  <si>
-    <t>RX PROMOCAO DE VENDAS E COMER</t>
-  </si>
-  <si>
     <t>AAZ COMERCIAL LTDA</t>
   </si>
   <si>
+    <t>Panificados</t>
+  </si>
+  <si>
+    <t>Leiloeiro Oficial</t>
+  </si>
+  <si>
+    <t>Reprografia</t>
+  </si>
+  <si>
+    <t>Gestão de Frota</t>
+  </si>
+  <si>
+    <t>Serviços de Engenharia</t>
+  </si>
+  <si>
+    <t>Resíduos Sólidos</t>
+  </si>
+  <si>
+    <t>Assistência Social</t>
+  </si>
+  <si>
+    <t>Licença de Software</t>
+  </si>
+  <si>
+    <t>Materiais de Tecnologia</t>
+  </si>
+  <si>
+    <t>Elevadores</t>
+  </si>
+  <si>
+    <t>Serviço Móvel</t>
+  </si>
+  <si>
+    <t>Montagem de Palanques</t>
+  </si>
+  <si>
+    <t>Locação de Móvel</t>
+  </si>
+  <si>
+    <t>Seguro Total</t>
+  </si>
+  <si>
+    <t>Cessão de Uso</t>
+  </si>
+  <si>
+    <t>Serviços de Limpeza</t>
+  </si>
+  <si>
     <t>Fornecimento de Energia</t>
   </si>
   <si>
-    <t>Assistência Social</t>
-  </si>
-  <si>
-    <t>Resíduos Sólidos</t>
-  </si>
-  <si>
-    <t>Serviços de Limpeza</t>
-  </si>
-  <si>
-    <t>Serviços de Engenharia</t>
-  </si>
-  <si>
-    <t>Gestão de Frota</t>
-  </si>
-  <si>
-    <t>Licença de Software</t>
-  </si>
-  <si>
-    <t>Central Telefônica</t>
-  </si>
-  <si>
-    <t>Materiais de Tecnologia</t>
-  </si>
-  <si>
-    <t>Elevadores</t>
-  </si>
-  <si>
-    <t>Serviço Móvel</t>
-  </si>
-  <si>
-    <t>Montagem de Palanques</t>
+    <t>TV por assinatura</t>
   </si>
   <si>
     <t>Serviço de Jardinagem</t>
   </si>
   <si>
-    <t>TV por assinatura</t>
-  </si>
-  <si>
-    <t>Cessão de Uso</t>
-  </si>
-  <si>
-    <t>Seguro Total</t>
-  </si>
-  <si>
-    <t>Locação de Móvel</t>
-  </si>
-  <si>
-    <t>Reprografia</t>
-  </si>
-  <si>
-    <t>Leiloeiro Oficial</t>
+    <t>Material de Expediente</t>
   </si>
   <si>
     <t>Peças de Elevadores</t>
   </si>
   <si>
-    <t>Panificados</t>
-  </si>
-  <si>
-    <t>Material de Expediente</t>
+    <t>Divisão de Manutenção e Reparo de PNR</t>
+  </si>
+  <si>
+    <t>Divisão de Gerência dos Créditos</t>
+  </si>
+  <si>
+    <t>Divisão de Conectividade de Sistemas de Informações</t>
+  </si>
+  <si>
+    <t>Divisão de Transporte</t>
+  </si>
+  <si>
+    <t>Divisão de Obras</t>
   </si>
   <si>
     <t>Divisão de Serviços Gerais</t>
@@ -463,61 +487,28 @@
     <t>Divisão de Assistência Social</t>
   </si>
   <si>
-    <t>Divisão de Obras</t>
-  </si>
-  <si>
-    <t>Divisão de Transporte</t>
-  </si>
-  <si>
-    <t>Divisão de Conectividade de Sistemas de Informações</t>
-  </si>
-  <si>
-    <t>Divisão de Segurança da Informação e Comunicações</t>
-  </si>
-  <si>
     <t>Divisão de Telefonia</t>
   </si>
   <si>
-    <t>Divisão de Manutenção e Reparo de PNR</t>
-  </si>
-  <si>
-    <t>Divisão de Gerência dos Créditos</t>
-  </si>
-  <si>
     <t>Divisão de Controle Patrimonial</t>
   </si>
   <si>
-    <t>SO</t>
-  </si>
-  <si>
-    <t>Mendonça</t>
-  </si>
-  <si>
-    <t>Messias</t>
-  </si>
-  <si>
-    <t>Posto Gestor</t>
-  </si>
-  <si>
-    <t>Posto Gestor Substituto</t>
-  </si>
-  <si>
-    <t>Posto Fiscal</t>
-  </si>
-  <si>
-    <t>Posto Fiscal Substituto</t>
-  </si>
-  <si>
-    <t>2T</t>
-  </si>
-  <si>
-    <t>Milliloi</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Siqueira Campos</t>
+    <t>CC (IM)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Guilherme Kirschner de Siqueira Campos</t>
+  </si>
+  <si>
+    <t>2t (AA)</t>
+  </si>
+  <si>
+    <t>Rogelio Millioli</t>
+  </si>
+  <si>
+    <t>Teste</t>
   </si>
 </sst>
 </file>
@@ -887,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -918,944 +909,944 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>160</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>161</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="K2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F3" t="s">
         <v>162</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J3" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F4" t="s">
         <v>162</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s">
         <v>162</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J5" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K5" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
         <v>162</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J6" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="F7" t="s">
         <v>162</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I7" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K7" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
         <v>162</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J8" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K8" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L8" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>162</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J9" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K9" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F10" t="s">
         <v>162</v>
       </c>
       <c r="G10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J10" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L10" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F11" t="s">
         <v>162</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J11" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L11" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F12" t="s">
         <v>162</v>
       </c>
       <c r="G12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="F13" t="s">
         <v>162</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I13" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J13" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K13" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L13" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="F14" t="s">
         <v>162</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J14" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
         <v>162</v>
       </c>
       <c r="G15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J15" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L15" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F16" t="s">
         <v>162</v>
       </c>
       <c r="G16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I16" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J16" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K16" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L16" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F17" t="s">
         <v>162</v>
       </c>
       <c r="G17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H17" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I17" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L17" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F18" t="s">
         <v>162</v>
       </c>
       <c r="G18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I18" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K18" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L18" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F19" t="s">
         <v>162</v>
       </c>
       <c r="G19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H19" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I19" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J19" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K19" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L19" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" t="s">
         <v>162</v>
       </c>
       <c r="G20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I20" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J20" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K20" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M20" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F21" t="s">
         <v>162</v>
       </c>
       <c r="G21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H21" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I21" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J21" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K21" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L21" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F22" t="s">
         <v>162</v>
       </c>
       <c r="G22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H22" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J22" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K22" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L22" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F23" t="s">
         <v>162</v>
       </c>
       <c r="G23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H23" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I23" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J23" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K23" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L23" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
         <v>153</v>
@@ -1864,203 +1855,203 @@
         <v>162</v>
       </c>
       <c r="G24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H24" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I24" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J24" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K24" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F25" t="s">
         <v>162</v>
       </c>
       <c r="G25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I25" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J25" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K25" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L25" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
         <v>162</v>
       </c>
       <c r="G26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I26" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J26" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K26" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L26" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
         <v>162</v>
       </c>
       <c r="G27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H27" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I27" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J27" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K27" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L27" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
         <v>162</v>
       </c>
       <c r="G28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H28" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I28" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J28" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K28" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L28" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E29" t="s">
         <v>149</v>
@@ -2069,1255 +2060,1255 @@
         <v>162</v>
       </c>
       <c r="G29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H29" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I29" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J29" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L29" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F30" t="s">
         <v>162</v>
       </c>
       <c r="G30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H30" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I30" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J30" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K30" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L30" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="F31" t="s">
         <v>162</v>
       </c>
       <c r="G31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I31" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J31" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K31" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L31" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F32" t="s">
         <v>162</v>
       </c>
       <c r="G32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H32" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I32" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J32" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L32" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F33" t="s">
         <v>162</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H33" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I33" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J33" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K33" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L33" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
         <v>162</v>
       </c>
       <c r="G34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I34" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J34" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K34" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L34" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F35" t="s">
         <v>162</v>
       </c>
       <c r="G35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H35" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I35" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J35" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K35" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L35" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E36" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F36" t="s">
         <v>162</v>
       </c>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H36" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I36" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J36" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L36" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
         <v>162</v>
       </c>
       <c r="G37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H37" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I37" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J37" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K37" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L37" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
         <v>162</v>
       </c>
       <c r="G38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H38" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I38" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J38" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K38" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L38" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F39" t="s">
         <v>162</v>
       </c>
       <c r="G39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H39" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I39" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J39" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K39" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L39" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
         <v>162</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H40" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I40" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J40" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K40" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L40" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M40" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F41" t="s">
         <v>162</v>
       </c>
       <c r="G41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H41" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I41" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J41" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K41" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L41" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M41" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F42" t="s">
         <v>162</v>
       </c>
       <c r="G42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I42" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J42" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K42" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L42" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M42" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F43" t="s">
         <v>162</v>
       </c>
       <c r="G43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H43" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I43" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J43" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K43" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L43" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F44" t="s">
         <v>162</v>
       </c>
       <c r="G44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H44" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I44" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J44" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K44" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L44" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E45" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F45" t="s">
         <v>162</v>
       </c>
       <c r="G45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H45" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I45" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J45" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K45" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L45" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M45" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F46" t="s">
         <v>162</v>
       </c>
       <c r="G46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H46" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I46" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J46" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K46" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L46" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F47" t="s">
         <v>162</v>
       </c>
       <c r="G47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H47" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I47" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J47" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K47" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L47" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M47" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F48" t="s">
         <v>162</v>
       </c>
       <c r="G48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H48" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I48" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J48" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K48" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L48" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M48" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E49" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="F49" t="s">
         <v>162</v>
       </c>
       <c r="G49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H49" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I49" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J49" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K49" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L49" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F50" t="s">
         <v>162</v>
       </c>
       <c r="G50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H50" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I50" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J50" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K50" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L50" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M50" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E51" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F51" t="s">
         <v>162</v>
       </c>
       <c r="G51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H51" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I51" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J51" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K51" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L51" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M51" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E52" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F52" t="s">
         <v>162</v>
       </c>
       <c r="G52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H52" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I52" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J52" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K52" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M52" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E53" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F53" t="s">
         <v>162</v>
       </c>
       <c r="G53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H53" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I53" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J53" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K53" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L53" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M53" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F54" t="s">
         <v>162</v>
       </c>
       <c r="G54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H54" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I54" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J54" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K54" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L54" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M54" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F55" t="s">
         <v>162</v>
       </c>
       <c r="G55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H55" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I55" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J55" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K55" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L55" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E56" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F56" t="s">
         <v>162</v>
       </c>
       <c r="G56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H56" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I56" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J56" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K56" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L56" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M56" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E57" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F57" t="s">
         <v>162</v>
       </c>
       <c r="G57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H57" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I57" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J57" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K57" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L57" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F58" t="s">
         <v>162</v>
       </c>
       <c r="G58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H58" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I58" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J58" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K58" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L58" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M58" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E59" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F59" t="s">
         <v>162</v>
       </c>
       <c r="G59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H59" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I59" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="J59" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="K59" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="L59" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="M59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit tabela de controle
</commit_message>
<xml_diff>
--- a/controle_contratos/Tabela_Gestores_Fiscais.xlsx
+++ b/controle_contratos/Tabela_Gestores_Fiscais.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/Programa PYQT6/pyqt6/controle_contratos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_23F921EDD1234E30692D4C261D7D54E979F84AF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F34EE89-4078-481A-A1B0-49C4E3996125}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="157">
   <si>
     <t>Número</t>
   </si>
@@ -61,177 +55,174 @@
     <t>Fiscal Substituto</t>
   </si>
   <si>
-    <t>87000/24-002/00</t>
+    <t>87000/21-120/00</t>
+  </si>
+  <si>
+    <t>87000/21-085/00</t>
+  </si>
+  <si>
+    <t>87000/21-086/00</t>
+  </si>
+  <si>
+    <t>87000/22-007/00</t>
+  </si>
+  <si>
+    <t>87000/23-073/00</t>
+  </si>
+  <si>
+    <t>87000/21-135/00</t>
   </si>
   <si>
     <t>87000/19-033/00</t>
   </si>
   <si>
-    <t>87000/22-007/00</t>
+    <t>87000/21-080/00</t>
+  </si>
+  <si>
+    <t>87000/21-084/00</t>
+  </si>
+  <si>
+    <t>87000/21-140/00</t>
+  </si>
+  <si>
+    <t>87000/23-099/00</t>
+  </si>
+  <si>
+    <t>87000/23-108/00</t>
+  </si>
+  <si>
+    <t>87000/23-088/00</t>
+  </si>
+  <si>
+    <t>87000/23-087/00</t>
+  </si>
+  <si>
+    <t>87000/20-082/00</t>
+  </si>
+  <si>
+    <t>87000/17-1532/00</t>
+  </si>
+  <si>
+    <t>87000/17-1531/00</t>
+  </si>
+  <si>
+    <t>87000/23-121/00</t>
+  </si>
+  <si>
+    <t>87000/23-115/00</t>
+  </si>
+  <si>
+    <t>87000/21-156/00</t>
+  </si>
+  <si>
+    <t>87000/19-058/00</t>
+  </si>
+  <si>
+    <t>87000/20-080/00</t>
   </si>
   <si>
     <t>87000/22-032/00</t>
   </si>
   <si>
-    <t>87000/21-084/00</t>
-  </si>
-  <si>
-    <t>87000/21-085/00</t>
-  </si>
-  <si>
-    <t>87000/21-086/00</t>
-  </si>
-  <si>
-    <t>87000/23-073/00</t>
-  </si>
-  <si>
-    <t>87000/21-135/00</t>
-  </si>
-  <si>
-    <t>87000/21-120/00</t>
-  </si>
-  <si>
-    <t>87000/23-087/00</t>
-  </si>
-  <si>
-    <t>87000/21-140/00</t>
-  </si>
-  <si>
-    <t>87000/23-099/00</t>
-  </si>
-  <si>
-    <t>87000/23-108/00</t>
-  </si>
-  <si>
-    <t>87000/23-088/00</t>
-  </si>
-  <si>
-    <t>87000/21-080/00</t>
-  </si>
-  <si>
-    <t>87000/20-082/00</t>
-  </si>
-  <si>
-    <t>87000/23-121/00</t>
-  </si>
-  <si>
-    <t>87000/23-115/00</t>
-  </si>
-  <si>
-    <t>87000/20-080/00</t>
-  </si>
-  <si>
-    <t>87000/21-156/00</t>
-  </si>
-  <si>
-    <t>87000/19-058/00</t>
+    <t>87000/22-009/00</t>
+  </si>
+  <si>
+    <t>87000/21-154/00</t>
+  </si>
+  <si>
+    <t>87000/19-057/00</t>
+  </si>
+  <si>
+    <t>87000/19-059/00</t>
+  </si>
+  <si>
+    <t>87000/23-043/00</t>
+  </si>
+  <si>
+    <t>87000/23-041/00</t>
+  </si>
+  <si>
+    <t>87000/23-040/00</t>
+  </si>
+  <si>
+    <t>87000/23-046/00</t>
+  </si>
+  <si>
+    <t>87000/23-037/00</t>
+  </si>
+  <si>
+    <t>87000/23-048/00</t>
+  </si>
+  <si>
+    <t>87000/23-033/00</t>
+  </si>
+  <si>
+    <t>87000/23-035/00</t>
+  </si>
+  <si>
+    <t>87000/23-045/00</t>
+  </si>
+  <si>
+    <t>87000/23-036/00</t>
+  </si>
+  <si>
+    <t>87000/23-032/00</t>
+  </si>
+  <si>
+    <t>87000/23-044/00</t>
+  </si>
+  <si>
+    <t>87000/23-042/00</t>
   </si>
   <si>
     <t>87000/21-109/00</t>
   </si>
   <si>
-    <t>87000/19-059/00</t>
-  </si>
-  <si>
-    <t>87000/17-1531/00</t>
-  </si>
-  <si>
-    <t>87000/17-1532/00</t>
-  </si>
-  <si>
-    <t>87000/19-057/00</t>
-  </si>
-  <si>
-    <t>87000/21-154/00</t>
-  </si>
-  <si>
-    <t>87000/22-009/00</t>
-  </si>
-  <si>
-    <t>87000/23-032/00</t>
-  </si>
-  <si>
-    <t>87000/23-036/00</t>
-  </si>
-  <si>
-    <t>87000/23-044/00</t>
-  </si>
-  <si>
-    <t>87000/23-045/00</t>
-  </si>
-  <si>
-    <t>87000/23-033/00</t>
-  </si>
-  <si>
-    <t>87000/23-035/00</t>
-  </si>
-  <si>
-    <t>87000/23-048/00</t>
-  </si>
-  <si>
-    <t>87000/23-037/00</t>
-  </si>
-  <si>
-    <t>87000/23-041/00</t>
-  </si>
-  <si>
-    <t>87000/23-040/00</t>
-  </si>
-  <si>
-    <t>87000/23-046/00</t>
-  </si>
-  <si>
-    <t>87000/23-043/00</t>
-  </si>
-  <si>
-    <t>87000/23-042/00</t>
+    <t>87000/23-076/00</t>
+  </si>
+  <si>
+    <t>87000/23-074/00</t>
+  </si>
+  <si>
+    <t>87000/23-082/00</t>
+  </si>
+  <si>
+    <t>87000/23-081/00</t>
+  </si>
+  <si>
+    <t>87000/23-031/00</t>
+  </si>
+  <si>
+    <t>87000/23-075/00</t>
+  </si>
+  <si>
+    <t>87000/23-078/00</t>
+  </si>
+  <si>
+    <t>87000/23-079/00</t>
+  </si>
+  <si>
+    <t>87000/23-080/00</t>
+  </si>
+  <si>
+    <t>87000/23-084/00</t>
+  </si>
+  <si>
+    <t>87000/23-085/00</t>
+  </si>
+  <si>
+    <t>87000/23-086/00</t>
+  </si>
+  <si>
+    <t>87000/23-098/00</t>
+  </si>
+  <si>
+    <t>87000/24-003/00</t>
   </si>
   <si>
     <t>87000/23-072/00</t>
   </si>
   <si>
-    <t>87000/23-076/00</t>
-  </si>
-  <si>
-    <t>87000/23-074/00</t>
-  </si>
-  <si>
-    <t>87000/23-082/00</t>
-  </si>
-  <si>
-    <t>87000/23-081/00</t>
-  </si>
-  <si>
-    <t>87000/23-031/00</t>
-  </si>
-  <si>
-    <t>87000/23-075/00</t>
-  </si>
-  <si>
-    <t>87000/23-078/00</t>
-  </si>
-  <si>
-    <t>87000/23-079/00</t>
-  </si>
-  <si>
-    <t>87000/23-080/00</t>
-  </si>
-  <si>
-    <t>87000/23-084/00</t>
-  </si>
-  <si>
-    <t>87000/23-085/00</t>
-  </si>
-  <si>
-    <t>87000/23-086/00</t>
-  </si>
-  <si>
-    <t>87000/23-098/00</t>
-  </si>
-  <si>
-    <t>87000/24-003/00</t>
-  </si>
-  <si>
     <t>87000/23-034/00</t>
   </si>
   <si>
@@ -241,126 +232,123 @@
     <t>Ata</t>
   </si>
   <si>
-    <t>UEDAMA COMERCIO DE PRODUTOS A</t>
+    <t>CLIAMA CLINICA DE ATENDIMENTO</t>
+  </si>
+  <si>
+    <t>HEIMAR-CONSTRUCOES E SERVICOS</t>
+  </si>
+  <si>
+    <t>TECNICALL ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>COPY LINE COMERCIO E SERVICOS</t>
+  </si>
+  <si>
+    <t>NORESA NOVO RIO ENERGIA E SER</t>
+  </si>
+  <si>
+    <t>VIVACE FISIOTERAPIA &amp; MEDICIN</t>
   </si>
   <si>
     <t>LUCIANO GONÇALVES BORBA ASSUNÇÃO</t>
   </si>
   <si>
-    <t>COPY LINE COMERCIO E SERVICOS</t>
+    <t>INTEGRAR - INSTITUTO DE REABI</t>
+  </si>
+  <si>
+    <t>ADTEL FACILITIES LTDA</t>
+  </si>
+  <si>
+    <t>PRATICAR CENTRO DE TREINAMENT</t>
+  </si>
+  <si>
+    <t>ELP COMERCIO DE EQUIPAMENTOS</t>
+  </si>
+  <si>
+    <t>OVER ELEVADORES LTDA</t>
+  </si>
+  <si>
+    <t>CLARO S.A.</t>
+  </si>
+  <si>
+    <t>MCR SISTEMAS E CONSULTORIA LT</t>
+  </si>
+  <si>
+    <t>STAR LOCACAO DE SERVICOS GERA</t>
+  </si>
+  <si>
+    <t>NEOENERGIA DISTRIBUICAO BRASI</t>
+  </si>
+  <si>
+    <t>ABRIGO DO MARINHEIRO</t>
+  </si>
+  <si>
+    <t>SEGUROS SURA S.A.</t>
+  </si>
+  <si>
+    <t>UNICA SERVICOS EM SAUDE LTDA</t>
+  </si>
+  <si>
+    <t>CAIXA ECONOMICA FEDERAL</t>
+  </si>
+  <si>
+    <t>PALCO LOCACAO LTDA</t>
   </si>
   <si>
     <t>NP3 COMERCIO E SERVICOS LTDA</t>
   </si>
   <si>
-    <t>ADTEL FACILITIES LTDA</t>
-  </si>
-  <si>
-    <t>HEIMAR-CONSTRUCOES E SERVICOS</t>
-  </si>
-  <si>
-    <t>TECNICALL ENGENHARIA LTDA</t>
-  </si>
-  <si>
-    <t>NORESA NOVO RIO ENERGIA E SER</t>
-  </si>
-  <si>
-    <t>VIVACE FISIOTERAPIA &amp; MEDICIN</t>
-  </si>
-  <si>
-    <t>CLIAMA CLINICA DE ATENDIMENTO</t>
-  </si>
-  <si>
-    <t>MCR SISTEMAS E CONSULTORIA LT</t>
-  </si>
-  <si>
-    <t>PRATICAR CENTRO DE TREINAMENT</t>
-  </si>
-  <si>
-    <t>ELP COMERCIO DE EQUIPAMENTOS</t>
-  </si>
-  <si>
-    <t>OVER ELEVADORES LTDA</t>
-  </si>
-  <si>
-    <t>CLARO S.A.</t>
-  </si>
-  <si>
-    <t>INTEGRAR - INSTITUTO DE REABI</t>
-  </si>
-  <si>
-    <t>STAR LOCACAO DE SERVICOS GERA</t>
-  </si>
-  <si>
-    <t>ABRIGO DO MARINHEIRO</t>
-  </si>
-  <si>
-    <t>SEGUROS SURA S.A.</t>
-  </si>
-  <si>
-    <t>PALCO LOCACAO LTDA</t>
-  </si>
-  <si>
-    <t>UNICA SERVICOS EM SAUDE LTDA</t>
-  </si>
-  <si>
-    <t>CAIXA ECONOMICA FEDERAL</t>
+    <t>ALFA E OMEGA  SERVICOS TERCEI</t>
+  </si>
+  <si>
+    <t>MARCIO ANDERSON RODRIGUES COM</t>
+  </si>
+  <si>
+    <t>BANCO BRADESCO S.A.</t>
+  </si>
+  <si>
+    <t>BANCO SANTANDER (BRASIL) S.A.</t>
+  </si>
+  <si>
+    <t>ALEGRENSE DISTRIBUIDORA E REP</t>
+  </si>
+  <si>
+    <t>DM COMERCIAL IMPORTADORA E EX</t>
+  </si>
+  <si>
+    <t>RAFA PAPER DISTRIBUIDORA LTDA</t>
+  </si>
+  <si>
+    <t>ART PAPER INDUSTRIA E COMERCI</t>
+  </si>
+  <si>
+    <t>RX PROMOCAO DE VENDAS E COMER</t>
+  </si>
+  <si>
+    <t>AMAZONAS COMERCIO DE ADESIVOS</t>
+  </si>
+  <si>
+    <t>VS - VIEIRA &amp; SANTOS COMERCIO</t>
+  </si>
+  <si>
+    <t>DAIANE DOS SANTOS MARTINS 133</t>
+  </si>
+  <si>
+    <t>LG COMERCIO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>LER - LIVRARIA E PAPELARIA LT</t>
+  </si>
+  <si>
+    <t>THIAGO CAETANIO DA SILVA 0549</t>
+  </si>
+  <si>
+    <t>SMART SOLUTIONS - SOLUCOES IN</t>
   </si>
   <si>
     <t>ANDRACON SERVICOS GERAIS LTDA</t>
   </si>
   <si>
-    <t>BANCO SANTANDER (BRASIL) S.A.</t>
-  </si>
-  <si>
-    <t>NEOENERGIA DISTRIBUICAO BRASI</t>
-  </si>
-  <si>
-    <t>BANCO BRADESCO S.A.</t>
-  </si>
-  <si>
-    <t>MARCIO ANDERSON RODRIGUES COM</t>
-  </si>
-  <si>
-    <t>ALFA E OMEGA  SERVICOS TERCEI</t>
-  </si>
-  <si>
-    <t>LER - LIVRARIA E PAPELARIA LT</t>
-  </si>
-  <si>
-    <t>LG COMERCIO E SERVICOS LTDA</t>
-  </si>
-  <si>
-    <t>THIAGO CAETANIO DA SILVA 0549</t>
-  </si>
-  <si>
-    <t>DAIANE DOS SANTOS MARTINS 133</t>
-  </si>
-  <si>
-    <t>AMAZONAS COMERCIO DE ADESIVOS</t>
-  </si>
-  <si>
-    <t>VS - VIEIRA &amp; SANTOS COMERCIO</t>
-  </si>
-  <si>
-    <t>RX PROMOCAO DE VENDAS E COMER</t>
-  </si>
-  <si>
-    <t>DM COMERCIAL IMPORTADORA E EX</t>
-  </si>
-  <si>
-    <t>RAFA PAPER DISTRIBUIDORA LTDA</t>
-  </si>
-  <si>
-    <t>ART PAPER INDUSTRIA E COMERCI</t>
-  </si>
-  <si>
-    <t>ALEGRENSE DISTRIBUIDORA E REP</t>
-  </si>
-  <si>
-    <t>SMART SOLUTIONS - SOLUCOES IN</t>
-  </si>
-  <si>
     <t>M&amp;M IMPORTACAO E ECOMMERCE DE</t>
   </si>
   <si>
@@ -403,119 +391,107 @@
     <t>AAZ COMERCIAL LTDA</t>
   </si>
   <si>
+    <t>Assistência Social</t>
+  </si>
+  <si>
+    <t>Serviços de Engenharia</t>
+  </si>
+  <si>
+    <t>Reprografia</t>
+  </si>
+  <si>
+    <t>Resíduos Sólidos</t>
+  </si>
+  <si>
+    <t>Leiloeiro Oficial</t>
+  </si>
+  <si>
+    <t>Materiais de Tecnologia</t>
+  </si>
+  <si>
+    <t>Elevadores</t>
+  </si>
+  <si>
+    <t>Serviço Móvel</t>
+  </si>
+  <si>
+    <t>Licença de Software</t>
+  </si>
+  <si>
+    <t>Montagem de Palanques</t>
+  </si>
+  <si>
+    <t>Fornecimento de Energia Elétrica</t>
+  </si>
+  <si>
+    <t>Fornecimento de Energia</t>
+  </si>
+  <si>
+    <t>Locação de Móvel</t>
+  </si>
+  <si>
+    <t>Seguro Total</t>
+  </si>
+  <si>
+    <t>Cessão de Uso</t>
+  </si>
+  <si>
+    <t>Gestão de Frota</t>
+  </si>
+  <si>
+    <t>Serviço de Jardinagem</t>
+  </si>
+  <si>
+    <t>TV por assinatura</t>
+  </si>
+  <si>
+    <t>Material de Expediente</t>
+  </si>
+  <si>
+    <t>Peças de Elevadores</t>
+  </si>
+  <si>
+    <t>Serviços de Limpeza</t>
+  </si>
+  <si>
     <t>Panificados</t>
   </si>
   <si>
-    <t>Leiloeiro Oficial</t>
-  </si>
-  <si>
-    <t>Reprografia</t>
-  </si>
-  <si>
-    <t>Gestão de Frota</t>
-  </si>
-  <si>
-    <t>Serviços de Engenharia</t>
-  </si>
-  <si>
-    <t>Resíduos Sólidos</t>
-  </si>
-  <si>
-    <t>Assistência Social</t>
-  </si>
-  <si>
-    <t>Licença de Software</t>
-  </si>
-  <si>
-    <t>Materiais de Tecnologia</t>
-  </si>
-  <si>
-    <t>Elevadores</t>
-  </si>
-  <si>
-    <t>Serviço Móvel</t>
-  </si>
-  <si>
-    <t>Montagem de Palanques</t>
-  </si>
-  <si>
-    <t>Locação de Móvel</t>
-  </si>
-  <si>
-    <t>Seguro Total</t>
-  </si>
-  <si>
-    <t>Cessão de Uso</t>
-  </si>
-  <si>
-    <t>Serviços de Limpeza</t>
-  </si>
-  <si>
-    <t>Fornecimento de Energia</t>
-  </si>
-  <si>
-    <t>TV por assinatura</t>
-  </si>
-  <si>
-    <t>Serviço de Jardinagem</t>
-  </si>
-  <si>
-    <t>Material de Expediente</t>
-  </si>
-  <si>
-    <t>Peças de Elevadores</t>
+    <t>Divisão de Assistência Social</t>
+  </si>
+  <si>
+    <t>Divisão de Obras</t>
+  </si>
+  <si>
+    <t>Divisão de Conectividade de Sistemas de Informações</t>
+  </si>
+  <si>
+    <t>Divisão de Serviços Gerais</t>
+  </si>
+  <si>
+    <t>Divisão de Gerência dos Créditos</t>
+  </si>
+  <si>
+    <t>Divisão de Telefonia</t>
   </si>
   <si>
     <t>Divisão de Manutenção e Reparo de PNR</t>
   </si>
   <si>
-    <t>Divisão de Gerência dos Créditos</t>
-  </si>
-  <si>
-    <t>Divisão de Conectividade de Sistemas de Informações</t>
-  </si>
-  <si>
     <t>Divisão de Transporte</t>
   </si>
   <si>
-    <t>Divisão de Obras</t>
-  </si>
-  <si>
-    <t>Divisão de Serviços Gerais</t>
-  </si>
-  <si>
-    <t>Divisão de Assistência Social</t>
-  </si>
-  <si>
-    <t>Divisão de Telefonia</t>
-  </si>
-  <si>
     <t>Divisão de Controle Patrimonial</t>
   </si>
   <si>
-    <t>CC (IM)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Guilherme Kirschner de Siqueira Campos</t>
-  </si>
-  <si>
-    <t>2t (AA)</t>
-  </si>
-  <si>
-    <t>Rogelio Millioli</t>
-  </si>
-  <si>
-    <t>Teste</t>
+    <t>TESTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,21 +554,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -630,7 +598,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -664,7 +632,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -699,10 +666,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -875,24 +841,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:K59"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
-    <col min="6" max="13" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="13" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,1114 +897,1114 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E23" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
         <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2048,40 +2012,40 @@
         <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2089,1226 +2053,1185 @@
         <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="F30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M36" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E37" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F37" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G37" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J37" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K37" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M37" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G38" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J38" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K38" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M39" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K40" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K41" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K42" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M42" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F43" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J43" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K43" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M44" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
         <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F45" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G45" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J45" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K45" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
         <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F46" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G46" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J46" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K46" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
         <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E47" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
         <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F48" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G48" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J48" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K48" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L48" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M48" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
         <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M49" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F50" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G50" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J50" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K50" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M50" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F51" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G51" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J51" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K51" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M51" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F52" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G52" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J52" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K52" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M52" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
         <v>120</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F53" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G53" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J53" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K53" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L53" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" t="s">
         <v>121</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F54" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G54" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J54" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K54" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M54" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C55" t="s">
         <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E55" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F55" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G55" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J55" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K55" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M55" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
         <v>123</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="E56" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F56" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G56" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J56" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K56" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M56" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F57" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G57" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J57" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K57" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M57" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="E58" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="F58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K58" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L58" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M58" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" t="s">
-        <v>126</v>
-      </c>
-      <c r="D59" t="s">
-        <v>146</v>
-      </c>
-      <c r="E59" t="s">
-        <v>156</v>
-      </c>
-      <c r="F59" t="s">
-        <v>162</v>
-      </c>
-      <c r="G59" t="s">
-        <v>162</v>
-      </c>
-      <c r="H59" t="s">
-        <v>158</v>
-      </c>
-      <c r="I59" t="s">
-        <v>158</v>
-      </c>
-      <c r="J59" t="s">
-        <v>162</v>
-      </c>
-      <c r="K59" t="s">
-        <v>162</v>
-      </c>
-      <c r="L59" t="s">
-        <v>158</v>
-      </c>
-      <c r="M59" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>